<commit_message>
commit new note in mid point and bressenham
</commit_message>
<xml_diff>
--- a/Bresenham_iterasi.xlsx
+++ b/Bresenham_iterasi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,10 +477,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
         <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -488,10 +488,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
         <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -499,10 +499,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
         <v>3</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -510,10 +510,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
         <v>3</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -521,10 +521,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
         <v>4</v>
-      </c>
-      <c r="C8" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -532,10 +532,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
         <v>5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -543,10 +543,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
         <v>5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -554,10 +554,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
         <v>6</v>
-      </c>
-      <c r="C11" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -565,10 +565,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -576,10 +576,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
         <v>7</v>
-      </c>
-      <c r="C13" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -587,10 +587,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="n">
         <v>8</v>
-      </c>
-      <c r="C14" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -598,10 +598,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -609,10 +609,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
         <v>9</v>
-      </c>
-      <c r="C16" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -620,10 +620,340 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="n">
         <v>10</v>
       </c>
-      <c r="C17" t="n">
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>23</v>
+      </c>
+      <c r="C25" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>24</v>
+      </c>
+      <c r="C26" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>25</v>
+      </c>
+      <c r="C27" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>27</v>
+      </c>
+      <c r="C29" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>28</v>
+      </c>
+      <c r="C30" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>29</v>
+      </c>
+      <c r="C31" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>31</v>
+      </c>
+      <c r="C33" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>32</v>
+      </c>
+      <c r="C34" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>33</v>
+      </c>
+      <c r="C35" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>34</v>
+      </c>
+      <c r="C36" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>35</v>
+      </c>
+      <c r="C37" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>36</v>
+      </c>
+      <c r="C38" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>37</v>
+      </c>
+      <c r="C39" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>38</v>
+      </c>
+      <c r="C40" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>39</v>
+      </c>
+      <c r="C41" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>40</v>
+      </c>
+      <c r="C42" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>41</v>
+      </c>
+      <c r="C43" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>42</v>
+      </c>
+      <c r="C44" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>43</v>
+      </c>
+      <c r="C45" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>44</v>
+      </c>
+      <c r="C46" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>45</v>
+      </c>
+      <c r="C47" t="n">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>